<commit_message>
3 and 4 th row
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1661ABE4-DED7-492F-B837-75415054E672}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65500309-3526-470A-A301-4E883DE82F40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>nisha</t>
+  </si>
+  <si>
+    <t>hgjkhk</t>
+  </si>
+  <si>
+    <t>gffgh</t>
+  </si>
+  <si>
+    <t>65h889</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +443,22 @@
       </c>
       <c r="B3">
         <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merged iwth the master
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">dumbi </t>
+  </si>
+  <si>
+    <t>djfkad</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -429,9 +432,17 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>98283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dumbi renamed as Yuktha
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -39,10 +39,10 @@
     <t>65h889</t>
   </si>
   <si>
-    <t xml:space="preserve">dumbi </t>
-  </si>
-  <si>
     <t>djfkad</t>
+  </si>
+  <si>
+    <t>Yuktha</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,7 +432,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>98283</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>

</xml_diff>